<commit_message>
Calibrated voltage outputs. Updated documentation.
</commit_message>
<xml_diff>
--- a/ADC Coefficients.xlsx
+++ b/ADC Coefficients.xlsx
@@ -402,7 +402,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +416,7 @@
       </c>
       <c r="B1">
         <f>(E1+E2*(E4/2)+E3/E4)*E5</f>
-        <v>99.44</v>
+        <v>100.8</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -431,13 +431,13 @@
       </c>
       <c r="B2">
         <f>(-E1+E2*(E4/2)-((2*E3)/E4))*E5</f>
-        <v>-118.16</v>
+        <v>-116.80000000000001</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2">
-        <v>6000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>